<commit_message>
altered R test file
</commit_message>
<xml_diff>
--- a/molgenis-scripts/src/test/resources/Rtest.xlsx
+++ b/molgenis-scripts/src/test/resources/Rtest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="840" yWindow="160" windowWidth="23160" windowHeight="17320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rtest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>variableA</t>
   </si>
@@ -82,10 +82,13 @@
     <t>id</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>decimal</t>
+  </si>
+  <si>
+    <t>AUTO</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -519,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1442,7 +1445,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1502,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1519,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -1536,7 +1539,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -1553,7 +1556,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -1570,7 +1573,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1578,8 +1581,8 @@
       <c r="G6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" t="b">
-        <v>1</v>
+      <c r="H6" t="s">
+        <v>21</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>

</xml_diff>